<commit_message>
added cross browser parallel suite xml, fixed DDT bugs
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-workspace\Framework_Handson_1\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0020EF5-0EDC-4C7A-8564-6152972F20CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF1BBD-2AFB-43B4-89A3-B0E3D7E182A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Google</t>
   </si>
@@ -52,6 +53,57 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>i5</t>
+  </si>
+  <si>
+    <t>i6</t>
+  </si>
+  <si>
+    <t>i7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.yahoo.com </t>
+  </si>
+  <si>
+    <t>https://www.gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.orkut.com</t>
+  </si>
+  <si>
+    <t>https://aot.edu.in</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>orkut</t>
+  </si>
+  <si>
+    <t>AOT</t>
+  </si>
+  <si>
+    <t>Facebook</t>
   </si>
 </sst>
 </file>
@@ -379,18 +431,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19B48F9-DE45-4D62-A3D4-DC67F6D01F34}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -428,8 +479,123 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{67E75693-8ED5-4580-B66B-D861C58DE053}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{0D51EB56-17BF-42FA-A955-1DCC34C97DC7}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5F141A83-FBCF-44D2-B621-FCBC2F187B86}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{3850FA0C-5D8F-4CF5-9414-D3A69F171B3A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72314F8E-AC56-40A2-9A7B-833436DA0792}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="58.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8794CEBE-BD31-416F-936A-24BD10938A86}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{3C5A31BB-13FD-41AB-A979-3E84B93747E5}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{FECA875A-4B2C-4706-9463-C2BE550FB96B}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{ED90037F-3D4A-4137-8F6C-71296196DB8A}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{695105FD-7FD4-4E02-8086-31442CECB7E2}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{681FB2AD-DF72-45F8-8B0F-0C2BDC34464D}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{21CF4A77-6805-4698-B7B3-1EE18E0A7676}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes to TestBase, refactoring browser setups
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-workspace\Framework_Handson_1\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF1BBD-2AFB-43B4-89A3-B0E3D7E182A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B3A28C-BEEC-4E06-BEDC-E1AFDA6F2700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>ee</t>
-  </si>
-  <si>
     <t>i4</t>
   </si>
   <si>
@@ -100,10 +97,13 @@
     <t>orkut</t>
   </si>
   <si>
-    <t>AOT</t>
-  </si>
-  <si>
     <t>Facebook</t>
+  </si>
+  <si>
+    <t>Academy</t>
+  </si>
+  <si>
+    <t>Yahoo</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +512,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -534,43 +534,43 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -578,13 +578,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>